<commit_message>
Se agregaron conclusiones y respuestas ACS
</commit_message>
<xml_diff>
--- a/RF-RNF.xlsx
+++ b/RF-RNF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Coronado\OneDrive\Escritorio\Prueba_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED2D5B5-0889-4493-896D-C91216B88BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F4621A-D3B8-4958-9972-418C377C03A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RF" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Metricas" sheetId="7" r:id="rId7"/>
     <sheet name="MTBF" sheetId="8" r:id="rId8"/>
     <sheet name="MTTR" sheetId="9" r:id="rId9"/>
+    <sheet name="Aplicación ACS" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="263">
   <si>
     <t>INSTRUCCIONES: Complete cada fila con la información del requisito funcional</t>
   </si>
@@ -359,9 +360,6 @@
   </si>
   <si>
     <t>Dado que un docente nuevo accede al sistema, cuando intenta subir un material por primera vez  la acción demora menos de 5 minutos sin consultar manuales.</t>
-  </si>
-  <si>
-    <t>Dado que es horario laboral(7:30-22:59), cuando los usuarios intentan acceder al sistema, entonces está disponible al menos el 99.5% del tiempo.</t>
   </si>
   <si>
     <t>RN-001</t>
@@ -742,12 +740,6 @@
     <t>tamaño del modulo</t>
   </si>
   <si>
-    <t>Reportes</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>MTBF</t>
   </si>
   <si>
@@ -764,13 +756,118 @@
   </si>
   <si>
     <t>Numero de fallas</t>
+  </si>
+  <si>
+    <t>Tipo de Riesgo</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>Por qué es un riesgo</t>
+  </si>
+  <si>
+    <t>Cómo A.C.S. lo corrige</t>
+  </si>
+  <si>
+    <t>Ambigüedad</t>
+  </si>
+  <si>
+    <t>“El sistema debe ser rápido”</t>
+  </si>
+  <si>
+    <t>No define qué significa “rápido”, dejando interpretación abierta</t>
+  </si>
+  <si>
+    <t>Desarrollo incorrecto, expectativas no cumplidas</t>
+  </si>
+  <si>
+    <t>FTR (First Time Review) para clarificar requisitos, métricas de tiempo, pruebas de rendimiento</t>
+  </si>
+  <si>
+    <t>Omisión</t>
+  </si>
+  <si>
+    <t>No se menciona cómo recuperar usuarios inactivos</t>
+  </si>
+  <si>
+    <t>Falta una función que puede ser necesaria</t>
+  </si>
+  <si>
+    <t>Usuarios bloqueados, insatisfacción</t>
+  </si>
+  <si>
+    <t>Validación de requisitos, pruebas de casos de uso completos</t>
+  </si>
+  <si>
+    <t>Requisitos no medibles</t>
+  </si>
+  <si>
+    <t>“La plataforma será fácil de usar”</t>
+  </si>
+  <si>
+    <t>No hay indicador cuantitativo para evaluar la facilidad</t>
+  </si>
+  <si>
+    <t>Difícil medir si se cumple, riesgo de baja usabilidad</t>
+  </si>
+  <si>
+    <t>Definición de métricas de usabilidad, encuestas, pruebas de usuario</t>
+  </si>
+  <si>
+    <t>Inconsistencia</t>
+  </si>
+  <si>
+    <t>“El administrador puede eliminar usuarios” vs “No se puede borrar ningún usuario”</t>
+  </si>
+  <si>
+    <t>Conflicto entre requisitos</t>
+  </si>
+  <si>
+    <t>Genera confusión en el desarrollo y errores de implementación</t>
+  </si>
+  <si>
+    <t>FTR, revisión cruzada de requisitos, pruebas de consistencia</t>
+  </si>
+  <si>
+    <t>Suposición no verificada</t>
+  </si>
+  <si>
+    <t>“Todos los estudiantes usan smartphones”</t>
+  </si>
+  <si>
+    <t>Supone que todos tienen dispositivos compatibles</t>
+  </si>
+  <si>
+    <t>Parte del público no podría acceder correctamente</t>
+  </si>
+  <si>
+    <t>Validación con encuestas, pruebas de acceso multiplataforma, ajustes según resultados</t>
+  </si>
+  <si>
+    <t>Inscripciones</t>
+  </si>
+  <si>
+    <t>Mayor</t>
+  </si>
+  <si>
+    <t>Tenemos una densidad de defectos del 7.5% cada 2000 LOC, lo cúal nos indica que nos falta pulir un poco de detalles para cumplir los estandares establecidos de calidad</t>
+  </si>
+  <si>
+    <t>Dado que es horario laboral(8:00-18:00), cuando los usuarios intentan acceder al sistema, entonces está disponible al menos el 99.5% del tiempo.</t>
+  </si>
+  <si>
+    <t>Tenemos como media de 40hrs de funcionamiento sin fallos, de un sistema el cual estará disponible en horario laboral por lo menos de 12hrs diarias y 60hrs semanales, lo cual nos indica que debemos mejorar el aspecto de confiabilidad</t>
+  </si>
+  <si>
+    <t>Tenemos como media de tiempo de reparación 30 minutos, lo cual es un tiempo bastante bueno para un sistema que necesita manejar grandes volumenes de información</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,8 +936,23 @@
       <name val="Monaco"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,6 +984,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,10 +1067,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -992,6 +1123,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1020,8 +1166,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Énfasis1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1302,7 +1452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1314,17 +1464,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="45">
       <c r="A2" s="2" t="s">
@@ -1625,12 +1775,136 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2297F75-29C8-4339-AB07-68779C8E6FD4}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60">
+      <c r="A2" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45">
+      <c r="A3" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60">
+      <c r="A4" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45">
+      <c r="A5" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60">
+      <c r="A6" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1642,15 +1916,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="45">
       <c r="A2" s="2" t="s">
@@ -1784,7 +2058,7 @@
         <v>45</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>104</v>
+        <v>260</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>64</v>
@@ -1813,12 +2087,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
@@ -1836,38 +2110,38 @@
     </row>
     <row r="3" spans="1:4" ht="38.25">
       <c r="A3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>106</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="38.25">
       <c r="A5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>50</v>
@@ -1878,10 +2152,10 @@
     </row>
     <row r="6" spans="1:4" ht="25.5">
       <c r="A6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>114</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>53</v>
@@ -1892,44 +2166,44 @@
     </row>
     <row r="7" spans="1:4" ht="38.25">
       <c r="A7" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>116</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25">
       <c r="A8" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>121</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>122</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1954,12 +2228,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
@@ -1977,44 +2251,44 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>126</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D5" s="13" t="s">
         <v>134</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2022,27 +2296,27 @@
         <v>71</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2050,41 +2324,41 @@
         <v>74</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>144</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="13" t="s">
         <v>151</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2092,13 +2366,13 @@
         <v>63</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="13" t="s">
         <v>154</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2106,13 +2380,13 @@
         <v>77</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="D12" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2120,13 +2394,13 @@
         <v>80</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>160</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2134,13 +2408,13 @@
         <v>81</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2155,8 +2429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2168,165 +2442,165 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="14" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="28.5">
+      <c r="A2" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.5">
-      <c r="A2" s="25" t="s">
+      <c r="C2" s="33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5">
+      <c r="A3" s="32"/>
+      <c r="B3" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="34"/>
+    </row>
+    <row r="4" spans="1:3" ht="28.5">
+      <c r="A4" s="32"/>
+      <c r="B4" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:3" ht="42.75">
+      <c r="A5" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5">
+      <c r="A6" s="32"/>
+      <c r="B6" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" ht="49.5" customHeight="1">
+      <c r="A7" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.5">
-      <c r="A3" s="25"/>
-      <c r="B3" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="27"/>
-    </row>
-    <row r="4" spans="1:3" ht="28.5">
-      <c r="A4" s="25"/>
-      <c r="B4" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4" s="28"/>
-    </row>
-    <row r="5" spans="1:3" ht="42.75">
-      <c r="A5" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="B7" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C7" s="36" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.5">
-      <c r="A6" s="25"/>
-      <c r="B6" s="8" t="s">
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="32"/>
+      <c r="B8" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="36"/>
+    </row>
+    <row r="9" spans="1:3" ht="49.5" customHeight="1">
+      <c r="A9" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="28"/>
-    </row>
-    <row r="7" spans="1:3" ht="49.5" customHeight="1">
-      <c r="A7" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.5">
-      <c r="A8" s="25"/>
-      <c r="B8" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="29"/>
-    </row>
-    <row r="9" spans="1:3" ht="49.5" customHeight="1">
-      <c r="A9" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="C10" s="36"/>
+    </row>
+    <row r="11" spans="1:3" ht="42.75">
+      <c r="A11" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C11" s="36" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="8" t="s">
+    <row r="12" spans="1:3" ht="28.5">
+      <c r="A12" s="32"/>
+      <c r="B12" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="36"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="29"/>
-    </row>
-    <row r="11" spans="1:3" ht="42.75">
-      <c r="A11" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.5">
-      <c r="A12" s="25"/>
-      <c r="B12" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="C12" s="29"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="29"/>
+      <c r="C13" s="36"/>
     </row>
     <row r="14" spans="1:3" ht="38.25">
       <c r="A14" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="42.75">
+      <c r="A15" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="B15" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="36" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="42.75">
-      <c r="A15" s="25" t="s">
+    <row r="16" spans="1:3" ht="28.5">
+      <c r="A16" s="32"/>
+      <c r="B16" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" s="29" t="s">
+      <c r="C16" s="36"/>
+    </row>
+    <row r="17" spans="1:3" ht="59.25" customHeight="1">
+      <c r="A17" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="36" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.5">
-      <c r="A16" s="25"/>
-      <c r="B16" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C16" s="29"/>
-    </row>
-    <row r="17" spans="1:3" ht="59.25" customHeight="1">
-      <c r="A17" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="10" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2367,13 +2641,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
@@ -2383,47 +2657,47 @@
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="33">
       <c r="A3" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="33">
       <c r="A4" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>203</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="33">
@@ -2431,33 +2705,33 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>206</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="33">
       <c r="A6" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>209</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="33">
@@ -2465,16 +2739,16 @@
         <v>77</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>212</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="33">
@@ -2482,16 +2756,16 @@
         <v>80</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>215</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2504,124 +2778,187 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C27583D-6BA7-4FBB-9D6A-53BF2B574A9B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="A6" sqref="A6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="24" t="s">
         <v>221</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="18" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="B2" s="1">
         <f>$C2/$D2</f>
-        <v>0.02</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="B3" s="1">
-        <f>$C3/$D3</f>
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>500</v>
-      </c>
+      <c r="A3" s="25"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:D8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C50D40-6EBF-4432-A06F-7B57EC71C6FC}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A4" sqref="A4:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>227</v>
+      <c r="A1" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
         <f>$B2/$C2</f>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:C8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A59A2C6-7E3A-4E70-B865-C0873A802D29}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>227</v>
+      </c>
+      <c r="D1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <f>(SUM($B2:$B5)/$C5)</f>
-        <v>37.5</v>
+        <f>(SUM($B2:$B5)/$D2)</f>
+        <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>40</v>
@@ -2629,8 +2966,12 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <f>MAX(C2:C5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>20</v>
@@ -2639,25 +2980,59 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
-      <c r="B5" s="1">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="20"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:D10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>